<commit_message>
GST Tools Flask App: GSTR-2 Excel Gen codes updated due to format change.
</commit_message>
<xml_diff>
--- a/GST_Tools_Flask_App/static/files/gstr2Atemplate.xlsx
+++ b/GST_Tools_Flask_App/static/files/gstr2Atemplate.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>SR NO</t>
   </si>
@@ -44,12 +44,6 @@
     <t>NAME</t>
   </si>
   <si>
-    <t>FILLING STATUS</t>
-  </si>
-  <si>
-    <t>PERIOD</t>
-  </si>
-  <si>
     <t>RATE</t>
   </si>
   <si>
@@ -72,13 +66,28 @@
   </si>
   <si>
     <t>Y/N</t>
+  </si>
+  <si>
+    <t>GSTR 3B FILED</t>
+  </si>
+  <si>
+    <t>GSTR 1 FILED</t>
+  </si>
+  <si>
+    <t>GSTR 1 FILLING DT</t>
+  </si>
+  <si>
+    <t>GSTR 1 PERIOD</t>
+  </si>
+  <si>
+    <t>Apr-19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +98,11 @@
     <font>
       <b/>
       <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -113,34 +127,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -448,7 +450,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -456,157 +458,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="9"/>
-    <col min="2" max="2" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="47.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="47.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:17" s="4" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="M1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="N1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="O1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="P1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="Q1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C2" s="2"/>
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="2">
-        <v>122019</v>
-      </c>
-      <c r="I2" s="2">
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C4" s="7"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="7"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C6" s="7"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C7" s="7"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C8" s="7"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C9" s="7"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C10" s="7"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C11" s="7"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C12" s="7"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C13" s="7"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C15" s="7"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C16" s="7"/>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C16" s="2"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="7"/>
+      <c r="C17" s="2"/>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="7"/>
+      <c r="C18" s="2"/>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="7"/>
+      <c r="C19" s="2"/>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="7"/>
+      <c r="C20" s="2"/>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="7"/>
+      <c r="C21" s="2"/>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="7"/>
+      <c r="C22" s="2"/>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" s="7"/>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" s="7"/>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" s="7"/>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C26" s="7"/>
+      <c r="C23" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>